<commit_message>
Botoes movidos para o grid e customizada aparencia
</commit_message>
<xml_diff>
--- a/Documentos/Anexos/40.xlsx
+++ b/Documentos/Anexos/40.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d37d5c4dc1513a8/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4718B23-2352-4841-9503-17B6211F907D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{0EB4BBEC-8C48-4763-97C9-49B8470AA67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EBDE4E73-C620-401C-8783-6F09639A2B20}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B9BF9D-2AB7-4727-92C7-A2671D95F7DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{91F777CB-D53F-4DEE-8921-ACD86291EAD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,22 +34,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>vigadexa</t>
-  </si>
-  <si>
-    <t>terolac</t>
-  </si>
-  <si>
-    <t>ecofilm</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+  <si>
+    <t>07h</t>
+  </si>
+  <si>
+    <t>09h</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>19h</t>
+  </si>
+  <si>
+    <t>21h</t>
+  </si>
+  <si>
+    <t>hidroclorotiazida</t>
+  </si>
+  <si>
+    <t>anlodipino</t>
+  </si>
+  <si>
+    <t>losartana</t>
+  </si>
+  <si>
+    <t>Cefalexina</t>
+  </si>
+  <si>
+    <t>Diosmina</t>
+  </si>
+  <si>
+    <t>Azitromicina</t>
+  </si>
+  <si>
+    <t>11h</t>
+  </si>
+  <si>
+    <t>23h</t>
+  </si>
+  <si>
+    <t>13h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +90,105 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -74,21 +196,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bom" xfId="1" builtinId="26"/>
+    <cellStyle name="Cálculo" xfId="4" builtinId="22"/>
+    <cellStyle name="Neutro" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ruim" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,78 +620,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BCCE73-A139-4917-96DC-2D4B4448D891}">
-  <dimension ref="F6:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991EC7A2-FC1A-4164-9B41-13438C7DED46}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:J10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
+    <col min="3" max="13" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="1" t="s">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="7" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="1" t="s">
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.875</v>
+      <c r="B11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A13:A14"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>